<commit_message>
Author : Ruchit Jain Description : Updated sql and database excel sheet for Profile Creation
</commit_message>
<xml_diff>
--- a/DB/DatabaseTPABReg.xlsx
+++ b/DB/DatabaseTPABReg.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="162">
   <si>
     <t>TrainingPartnerOrganizationDetails</t>
   </si>
@@ -39,24 +39,12 @@
     <t>pincode</t>
   </si>
   <si>
-    <t>landlineNumber1</t>
-  </si>
-  <si>
-    <t>landlineNumber2</t>
-  </si>
-  <si>
     <t>faxNumber</t>
   </si>
   <si>
-    <t>websites(comma seperated)</t>
-  </si>
-  <si>
     <t>yearOfEstablishment</t>
   </si>
   <si>
-    <t>NSDCFunded</t>
-  </si>
-  <si>
     <t>selfOwnedInstitution</t>
   </si>
   <si>
@@ -72,15 +60,9 @@
     <t>tanNumber</t>
   </si>
   <si>
-    <t>instituteReceivedAnyGrant(*)</t>
-  </si>
-  <si>
     <t>priorExperienceOfInstitutionInSkillDevelopment</t>
   </si>
   <si>
-    <t>anyPriorExperienceOfInstitutionInSkillTraining(*)</t>
-  </si>
-  <si>
     <t>TrainingPartnerCenterLevelDetails</t>
   </si>
   <si>
@@ -96,9 +78,6 @@
     <t>numberOfPermanentOfficeStaff</t>
   </si>
   <si>
-    <t>numberOfTemporaryOfficeStaff</t>
-  </si>
-  <si>
     <t>numberOfPermanentLabAssistants</t>
   </si>
   <si>
@@ -165,9 +144,6 @@
     <t>numberOfNonTechnicalBooks</t>
   </si>
   <si>
-    <t>numberOfMagazine</t>
-  </si>
-  <si>
     <t>numberOfDailies</t>
   </si>
   <si>
@@ -195,9 +171,6 @@
     <t>remarksOnStudentAdmissionDetails</t>
   </si>
   <si>
-    <t>InstituteGrant</t>
-  </si>
-  <si>
     <t>nameOfMinistry</t>
   </si>
   <si>
@@ -207,9 +180,6 @@
     <t>remarks</t>
   </si>
   <si>
-    <t>InstituteRecognition</t>
-  </si>
-  <si>
     <t>nameOfRecognizingBody</t>
   </si>
   <si>
@@ -219,21 +189,12 @@
     <t>yearOfRecognition</t>
   </si>
   <si>
-    <t>validityOfRecognition(varchar)</t>
-  </si>
-  <si>
-    <t>PriorExperienceInSkillTraining</t>
-  </si>
-  <si>
     <t>courseName</t>
   </si>
   <si>
     <t>numberOfStudentsInEachBatch</t>
   </si>
   <si>
-    <t>type(Management,TrainingStaff,Officials)</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -270,15 +231,6 @@
     <t>int(6)</t>
   </si>
   <si>
-    <t>int(11)</t>
-  </si>
-  <si>
-    <t>int(13)</t>
-  </si>
-  <si>
-    <t>int(14)</t>
-  </si>
-  <si>
     <t>varchar(100)</t>
   </si>
   <si>
@@ -294,27 +246,15 @@
     <t>varchar(10)</t>
   </si>
   <si>
-    <t>int(10)</t>
-  </si>
-  <si>
     <t>decimal(6,2)</t>
   </si>
   <si>
-    <t>turnOverOfInstitution   (In lakhs)</t>
-  </si>
-  <si>
     <t>varchar(3)</t>
   </si>
   <si>
     <t>varchar(20)</t>
   </si>
   <si>
-    <t>areaOfInstitute ( in sqft)</t>
-  </si>
-  <si>
-    <t>sizeOfClassrooms ( in sqft)</t>
-  </si>
-  <si>
     <t>varchar(1000)</t>
   </si>
   <si>
@@ -330,27 +270,12 @@
     <t>concessionPolicy</t>
   </si>
   <si>
-    <t>int(15)</t>
-  </si>
-  <si>
-    <t>ManagementAndStaffAndOfficialsDetails</t>
-  </si>
-  <si>
-    <t>(To be inserted by us)</t>
-  </si>
-  <si>
     <t>from user table only</t>
   </si>
   <si>
-    <t>can be tinyint</t>
-  </si>
-  <si>
     <t>qualificationPacksAnnexurePath</t>
   </si>
   <si>
-    <t>NSDCCertificatePath</t>
-  </si>
-  <si>
     <t>selfOwnedInstitutionAnnexurePath</t>
   </si>
   <si>
@@ -378,9 +303,6 @@
     <t>labPicsPath</t>
   </si>
   <si>
-    <t>WorkshopPicsPath</t>
-  </si>
-  <si>
     <t>mandatoryToolKitAnnexurePath</t>
   </si>
   <si>
@@ -393,30 +315,12 @@
     <t>certificatePath</t>
   </si>
   <si>
-    <t>mediumOfInstructions(comma seperated)</t>
-  </si>
-  <si>
-    <t>qualificationPacks (comma separated)</t>
-  </si>
-  <si>
-    <t>yearOfEstablishment (yyyy)</t>
-  </si>
-  <si>
     <t>mobileNumber</t>
   </si>
   <si>
     <t>alternateMobileNumber</t>
   </si>
   <si>
-    <t>insituteReceivedAnyRecognition(*)</t>
-  </si>
-  <si>
-    <t>trainingPartnerCenterId (PK)</t>
-  </si>
-  <si>
-    <t>applicationId(FK)</t>
-  </si>
-  <si>
     <t>numberOfBatchesPerYear</t>
   </si>
   <si>
@@ -432,12 +336,6 @@
     <t>validityOfRecognition</t>
   </si>
   <si>
-    <t>NameOfRecognitionBody</t>
-  </si>
-  <si>
-    <t>RecognitionNumber</t>
-  </si>
-  <si>
     <t>numberOfTechnicalAssessors</t>
   </si>
   <si>
@@ -468,60 +366,12 @@
     <t>jobRoleCode</t>
   </si>
   <si>
-    <t>district</t>
-  </si>
-  <si>
-    <t>RegionalOfficeDetails</t>
-  </si>
-  <si>
     <t>alternateContactNumber</t>
   </si>
   <si>
-    <t>instituteGrantId(PK)</t>
-  </si>
-  <si>
-    <t>instituteRecognitionId(PK)</t>
-  </si>
-  <si>
-    <t>priorExperienceInSkillTrainingId(PK)</t>
-  </si>
-  <si>
-    <t>ManagementAndStaffId (PK)</t>
-  </si>
-  <si>
     <t>Added field to distinguish OH,AC,POC details of each center</t>
   </si>
   <si>
-    <t>trainingPartnerCenterId (FK)</t>
-  </si>
-  <si>
-    <t>trainingPartnerRegistrationId(FK)</t>
-  </si>
-  <si>
-    <t>trainingPartnerRegistrationId(PK)</t>
-  </si>
-  <si>
-    <t>assessmentBodyRegistrationId(PK)</t>
-  </si>
-  <si>
-    <t>assessmentExperienceId(PK)</t>
-  </si>
-  <si>
-    <t>assessmentBodyRegistrationId(FK)</t>
-  </si>
-  <si>
-    <t>directorsAndManagementId(PK)</t>
-  </si>
-  <si>
-    <t>assessmentStaffId(PK)</t>
-  </si>
-  <si>
-    <t>regionalOfficeId(PK)</t>
-  </si>
-  <si>
-    <t>affiliationId(PK)</t>
-  </si>
-  <si>
     <t>nameOfSectorSkillCouncil</t>
   </si>
   <si>
@@ -537,7 +387,121 @@
     <t>alternateLandlineNumber</t>
   </si>
   <si>
-    <t>userId</t>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>websites</t>
+  </si>
+  <si>
+    <t>qualificationPacks</t>
+  </si>
+  <si>
+    <t>nSDCFunded</t>
+  </si>
+  <si>
+    <t>nSDCFundedCertificatePath</t>
+  </si>
+  <si>
+    <t>mediumOfInstructions</t>
+  </si>
+  <si>
+    <t>turnOverOfInstitution</t>
+  </si>
+  <si>
+    <t>instituteReceivedAnyGrant</t>
+  </si>
+  <si>
+    <t>instituteReceivedAnyRecognition</t>
+  </si>
+  <si>
+    <t>anyPriorExperienceOfInstitutionInSkillTraining</t>
+  </si>
+  <si>
+    <t>trainingPartnerRegistrationId</t>
+  </si>
+  <si>
+    <t>applicationId</t>
+  </si>
+  <si>
+    <t>trainingPartnerCenterId</t>
+  </si>
+  <si>
+    <t>numberOftemporaryOfficeManager</t>
+  </si>
+  <si>
+    <t>areaOfInstitute</t>
+  </si>
+  <si>
+    <t>sizeOfClassrooms</t>
+  </si>
+  <si>
+    <t>workshopPicsPath</t>
+  </si>
+  <si>
+    <t>varchar(5)</t>
+  </si>
+  <si>
+    <t>numberOfMagazines</t>
+  </si>
+  <si>
+    <t>instituteGrantId</t>
+  </si>
+  <si>
+    <t>TrainingPartnerInstituteGrant</t>
+  </si>
+  <si>
+    <t>TrainingPartnerInstituteRecognition</t>
+  </si>
+  <si>
+    <t>instituteRecognitionId</t>
+  </si>
+  <si>
+    <t>TrainingPartnerPriorExperienceInSkillTraining</t>
+  </si>
+  <si>
+    <t>priorExperienceInSkillTrainingId</t>
+  </si>
+  <si>
+    <t>TrainingPartnerManagementAndStaffAndOfficialsDetails</t>
+  </si>
+  <si>
+    <t>managementAndStaffId</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>(To be inserted by us)(Management,TrainingStaff,Officials)</t>
+  </si>
+  <si>
+    <t>assessmentBodyRegistrationId</t>
+  </si>
+  <si>
+    <t>AssessmentBodyRecognitions</t>
+  </si>
+  <si>
+    <t>assessmentBodyRecognitionId</t>
+  </si>
+  <si>
+    <t>nameOfRecognitionBody</t>
+  </si>
+  <si>
+    <t>assessmentExperienceId</t>
+  </si>
+  <si>
+    <t>directorsAndManagementId</t>
+  </si>
+  <si>
+    <t>assessmentStaffId</t>
+  </si>
+  <si>
+    <t>AssessmentBodyRegionalOfficeDetails</t>
+  </si>
+  <si>
+    <t>regionalOfficeId</t>
+  </si>
+  <si>
+    <t>affiliationId</t>
   </si>
 </sst>
 </file>
@@ -660,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -672,6 +636,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -975,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -989,1012 +956,1001 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25.8">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>114</v>
-      </c>
-      <c r="B31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>17</v>
-      </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="25.8">
-      <c r="A43" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="12"/>
+      <c r="A43" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="13"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="10" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B59" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>27</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="B61" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="B70" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B71" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="B73" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>50</v>
+        <v>141</v>
       </c>
       <c r="B82" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="B84" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B85" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B86" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B88" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>50</v>
+      </c>
+      <c r="B95" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="25.8">
-      <c r="A97" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B97" s="12"/>
+      <c r="A97" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B97" s="13"/>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="2" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="10" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B101" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B102" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B103" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="25.8">
-      <c r="A106" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B106" s="12"/>
+      <c r="A106" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B106" s="13"/>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="10" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B110" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B111" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
+        <v>105</v>
+      </c>
+      <c r="B113" t="s">
         <v>67</v>
       </c>
-      <c r="B113" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="116" spans="1:2" ht="25.8">
-      <c r="A116" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B116" s="12"/>
+      <c r="A116" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B116" s="13"/>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="10" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B120" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="B121" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B122" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="25.8">
-      <c r="A125" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B125" s="12"/>
+      <c r="A125" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B125" s="13"/>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1"/>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="10" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="10" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C129" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="4" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C130" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B131" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B132" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B133" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B134" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B135" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B136" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B137" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="B138" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="B139" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="25.8">
-      <c r="A141" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B141" s="13"/>
+      <c r="A141" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B141" s="14"/>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="7" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2002,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="B145" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2010,7 +1966,7 @@
         <v>2</v>
       </c>
       <c r="B146" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2018,7 +1974,7 @@
         <v>3</v>
       </c>
       <c r="B147" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2026,7 +1982,7 @@
         <v>4</v>
       </c>
       <c r="B148" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2034,7 +1990,7 @@
         <v>5</v>
       </c>
       <c r="B149" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2042,501 +1998,520 @@
         <v>6</v>
       </c>
       <c r="B150" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="B151" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="B152" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="B153" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="B154" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B155" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="B156" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B157" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="B158" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B159" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="B160" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B161" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="B162" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="B163" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="B164" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="B165" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="B166" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2">
-      <c r="A167" t="s">
-        <v>137</v>
-      </c>
-      <c r="B167" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2">
-      <c r="A168" t="s">
-        <v>140</v>
-      </c>
-      <c r="B168" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2">
-      <c r="A169" t="s">
-        <v>141</v>
-      </c>
-      <c r="B169" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2">
-      <c r="A170" t="s">
-        <v>142</v>
-      </c>
-      <c r="B170" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="25.8">
-      <c r="A173" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B173" s="13"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="25.8">
+      <c r="A169" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B169" s="14"/>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>155</v>
+      </c>
+      <c r="B173" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>55</v>
+      </c>
+      <c r="B174" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="175" spans="1:2">
-      <c r="A175" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>79</v>
+      <c r="A175" t="s">
+        <v>56</v>
+      </c>
+      <c r="B175" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="176" spans="1:2">
-      <c r="A176" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B176" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2">
-      <c r="A177" t="s">
-        <v>144</v>
-      </c>
-      <c r="B177" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2">
-      <c r="A178" t="s">
-        <v>145</v>
-      </c>
-      <c r="B178" t="s">
-        <v>79</v>
+      <c r="A176" t="s">
+        <v>105</v>
+      </c>
+      <c r="B176" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="25.8">
-      <c r="A181" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B181" s="13"/>
+      <c r="A181" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B181" s="14"/>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B183" s="7" t="s">
-        <v>79</v>
+        <v>156</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="9" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B185" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="B186" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2">
-      <c r="A187" t="s">
-        <v>75</v>
-      </c>
-      <c r="B187" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2">
-      <c r="A188" t="s">
-        <v>74</v>
-      </c>
-      <c r="B188" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2">
-      <c r="A189" t="s">
-        <v>76</v>
-      </c>
-      <c r="B189" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2">
-      <c r="A190" t="s">
-        <v>78</v>
-      </c>
-      <c r="B190" t="s">
-        <v>90</v>
-      </c>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="25.8">
+      <c r="A189" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B189" s="11"/>
     </row>
     <row r="191" spans="1:2">
-      <c r="A191" t="s">
+      <c r="A191" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>59</v>
+      </c>
+      <c r="B193" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>60</v>
+      </c>
+      <c r="B194" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>62</v>
+      </c>
+      <c r="B195" t="s">
         <v>123</v>
       </c>
-      <c r="B191" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="25.8">
-      <c r="A193" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B193" s="13"/>
-    </row>
-    <row r="195" spans="1:2">
-      <c r="A195" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B195" s="7" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="196" spans="1:2">
-      <c r="A196" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B196" s="6" t="s">
-        <v>79</v>
+      <c r="A196" t="s">
+        <v>61</v>
+      </c>
+      <c r="B196" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>148</v>
+        <v>63</v>
       </c>
       <c r="B197" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="B198" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B199" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2">
-      <c r="A200" t="s">
-        <v>75</v>
-      </c>
-      <c r="B200" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2">
-      <c r="A201" t="s">
-        <v>74</v>
-      </c>
-      <c r="B201" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2">
-      <c r="A202" t="s">
-        <v>5</v>
-      </c>
-      <c r="B202" t="s">
-        <v>81</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="25.8">
+      <c r="A201" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B201" s="11"/>
     </row>
     <row r="203" spans="1:2">
-      <c r="A203" t="s">
-        <v>150</v>
-      </c>
-      <c r="B203" t="s">
-        <v>81</v>
+      <c r="A203" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="204" spans="1:2">
-      <c r="A204" t="s">
-        <v>76</v>
-      </c>
-      <c r="B204" t="s">
-        <v>87</v>
+      <c r="A204" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B205" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B206" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="B207" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="25.8">
-      <c r="A210" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B210" s="13"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>62</v>
+      </c>
+      <c r="B208" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>61</v>
+      </c>
+      <c r="B209" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>5</v>
+      </c>
+      <c r="B210" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>4</v>
+      </c>
+      <c r="B211" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="212" spans="1:2">
-      <c r="A212" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B212" s="7" t="s">
-        <v>79</v>
+      <c r="A212" t="s">
+        <v>63</v>
+      </c>
+      <c r="B212" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="213" spans="1:2">
-      <c r="A213" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B213" s="6" t="s">
-        <v>79</v>
+      <c r="A213" t="s">
+        <v>65</v>
+      </c>
+      <c r="B213" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B214" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
+        <v>98</v>
+      </c>
+      <c r="B215" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="25.8">
+      <c r="A218" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B218" s="11"/>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>3</v>
+      </c>
+      <c r="B222" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
         <v>5</v>
       </c>
-      <c r="B215" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2">
-      <c r="A216" t="s">
+      <c r="B223" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
         <v>6</v>
       </c>
-      <c r="B216" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2">
-      <c r="A217" t="s">
-        <v>75</v>
-      </c>
-      <c r="B217" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2">
-      <c r="A218" t="s">
-        <v>152</v>
-      </c>
-      <c r="B218" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="25.8">
-      <c r="A221" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="B221" s="13"/>
-    </row>
-    <row r="223" spans="1:2">
-      <c r="A223" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B223" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2">
-      <c r="A224" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B224" s="6" t="s">
-        <v>79</v>
+      <c r="B224" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>168</v>
+        <v>62</v>
       </c>
       <c r="B225" t="s">
-        <v>169</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>116</v>
+      </c>
+      <c r="B226" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="25.8">
+      <c r="A229" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B229" s="11"/>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>118</v>
+      </c>
+      <c r="B233" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A221:B221"/>
-    <mergeCell ref="A210:B210"/>
     <mergeCell ref="A116:B116"/>
     <mergeCell ref="A125:B125"/>
     <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A173:B173"/>
     <mergeCell ref="A181:B181"/>
-    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>